<commit_message>
Add Set default Setting Button
</commit_message>
<xml_diff>
--- a/Spr/xls_forms/F22_I.xlsx
+++ b/Spr/xls_forms/F22_I.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FC6A8A-0490-48FB-84D7-05D6AEE59D05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639FD8F6-97D5-48C2-926E-DCF9F5A93754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1270,6 +1270,75 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1297,77 +1366,8 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1799,10 +1799,10 @@
   <dimension ref="A1:EA187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="AQ33" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AH42" sqref="AH42:AX48"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,76 +1815,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:131" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="96" t="s">
+      <c r="A1" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="96" t="s">
+      <c r="C1" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="96" t="s">
+      <c r="D1" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="96" t="s">
+      <c r="E1" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="96" t="s">
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="97"/>
-      <c r="R1" s="97"/>
-      <c r="S1" s="97"/>
-      <c r="T1" s="97"/>
-      <c r="U1" s="97"/>
-      <c r="V1" s="97"/>
-      <c r="W1" s="96" t="s">
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="X1" s="103"/>
-      <c r="Y1" s="103"/>
-      <c r="Z1" s="103"/>
-      <c r="AA1" s="103"/>
-      <c r="AB1" s="103"/>
-      <c r="AC1" s="103"/>
-      <c r="AD1" s="103"/>
-      <c r="AE1" s="103"/>
-      <c r="AF1" s="103"/>
-      <c r="AG1" s="103"/>
-      <c r="AH1" s="103"/>
-      <c r="AI1" s="103"/>
-      <c r="AJ1" s="104" t="s">
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
+      <c r="AG1" s="78"/>
+      <c r="AH1" s="78"/>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="AK1" s="103"/>
-      <c r="AL1" s="103"/>
-      <c r="AM1" s="103"/>
-      <c r="AN1" s="105" t="s">
+      <c r="AK1" s="78"/>
+      <c r="AL1" s="78"/>
+      <c r="AM1" s="78"/>
+      <c r="AN1" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="AO1" s="106"/>
-      <c r="AP1" s="106"/>
-      <c r="AQ1" s="106"/>
-      <c r="AR1" s="96" t="s">
+      <c r="AO1" s="81"/>
+      <c r="AP1" s="81"/>
+      <c r="AQ1" s="81"/>
+      <c r="AR1" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="AS1" s="97"/>
-      <c r="AT1" s="97"/>
-      <c r="AU1" s="97"/>
-      <c r="AV1" s="97"/>
-      <c r="AW1" s="97"/>
-      <c r="AX1" s="97"/>
+      <c r="AS1" s="76"/>
+      <c r="AT1" s="76"/>
+      <c r="AU1" s="76"/>
+      <c r="AV1" s="76"/>
+      <c r="AW1" s="76"/>
+      <c r="AX1" s="76"/>
       <c r="AY1" s="89" t="s">
         <v>91</v>
       </c>
@@ -1970,118 +1970,118 @@
       <c r="EA1" s="1"/>
     </row>
     <row r="2" spans="1:131" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="107"/>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96" t="s">
+      <c r="A2" s="77"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="96" t="s">
+      <c r="F2" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="96" t="s">
+      <c r="G2" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="96" t="s">
+      <c r="H2" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="96" t="s">
+      <c r="I2" s="75" t="s">
         <v>96</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="96" t="s">
+      <c r="K2" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="96" t="s">
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="O2" s="96" t="s">
+      <c r="O2" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="P2" s="97"/>
-      <c r="Q2" s="96" t="s">
+      <c r="P2" s="76"/>
+      <c r="Q2" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="R2" s="96" t="s">
+      <c r="R2" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="S2" s="96" t="s">
+      <c r="S2" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="T2" s="96" t="s">
+      <c r="T2" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="U2" s="96" t="s">
+      <c r="U2" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="V2" s="96" t="s">
+      <c r="V2" s="75" t="s">
         <v>104</v>
       </c>
-      <c r="W2" s="96" t="s">
+      <c r="W2" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="X2" s="96" t="s">
+      <c r="X2" s="75" t="s">
         <v>106</v>
       </c>
-      <c r="Y2" s="96" t="s">
+      <c r="Y2" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="Z2" s="96" t="s">
+      <c r="Z2" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="AA2" s="96" t="s">
+      <c r="AA2" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="AB2" s="97"/>
-      <c r="AC2" s="97"/>
-      <c r="AD2" s="96" t="s">
+      <c r="AB2" s="76"/>
+      <c r="AC2" s="76"/>
+      <c r="AD2" s="75" t="s">
         <v>109</v>
       </c>
-      <c r="AE2" s="102" t="s">
+      <c r="AE2" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="AF2" s="103"/>
-      <c r="AG2" s="103"/>
-      <c r="AH2" s="103"/>
-      <c r="AI2" s="103"/>
-      <c r="AJ2" s="96" t="s">
+      <c r="AF2" s="78"/>
+      <c r="AG2" s="78"/>
+      <c r="AH2" s="78"/>
+      <c r="AI2" s="78"/>
+      <c r="AJ2" s="75" t="s">
         <v>110</v>
       </c>
-      <c r="AK2" s="96" t="s">
+      <c r="AK2" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="AL2" s="97"/>
-      <c r="AM2" s="97"/>
-      <c r="AN2" s="96" t="s">
+      <c r="AL2" s="76"/>
+      <c r="AM2" s="76"/>
+      <c r="AN2" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="AO2" s="96" t="s">
+      <c r="AO2" s="75" t="s">
         <v>112</v>
       </c>
-      <c r="AP2" s="96" t="s">
+      <c r="AP2" s="75" t="s">
         <v>113</v>
       </c>
-      <c r="AQ2" s="96" t="s">
+      <c r="AQ2" s="75" t="s">
         <v>114</v>
       </c>
-      <c r="AR2" s="96" t="s">
+      <c r="AR2" s="75" t="s">
         <v>115</v>
       </c>
-      <c r="AS2" s="96" t="s">
+      <c r="AS2" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="AT2" s="97"/>
-      <c r="AU2" s="97"/>
-      <c r="AV2" s="97"/>
-      <c r="AW2" s="96" t="s">
+      <c r="AT2" s="76"/>
+      <c r="AU2" s="76"/>
+      <c r="AV2" s="76"/>
+      <c r="AW2" s="75" t="s">
         <v>116</v>
       </c>
-      <c r="AX2" s="98" t="s">
+      <c r="AX2" s="83" t="s">
         <v>117</v>
       </c>
       <c r="AY2" s="89"/>
@@ -2167,96 +2167,96 @@
       <c r="EA2" s="1"/>
     </row>
     <row r="3" spans="1:131" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="107"/>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96" t="s">
+      <c r="A3" s="77"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75" t="s">
         <v>118</v>
       </c>
-      <c r="K3" s="96" t="s">
+      <c r="K3" s="75" t="s">
         <v>119</v>
       </c>
-      <c r="L3" s="96" t="s">
+      <c r="L3" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="96" t="s">
+      <c r="M3" s="76"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="P3" s="96" t="s">
+      <c r="P3" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="97"/>
-      <c r="T3" s="97"/>
-      <c r="U3" s="97"/>
-      <c r="V3" s="97"/>
-      <c r="W3" s="97"/>
-      <c r="X3" s="97"/>
-      <c r="Y3" s="97"/>
-      <c r="Z3" s="97"/>
-      <c r="AA3" s="96" t="s">
+      <c r="Q3" s="76"/>
+      <c r="R3" s="76"/>
+      <c r="S3" s="76"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="76"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="76"/>
+      <c r="Z3" s="76"/>
+      <c r="AA3" s="75" t="s">
         <v>123</v>
       </c>
-      <c r="AB3" s="96" t="s">
+      <c r="AB3" s="75" t="s">
         <v>124</v>
       </c>
-      <c r="AC3" s="96" t="s">
+      <c r="AC3" s="75" t="s">
         <v>125</v>
       </c>
-      <c r="AD3" s="97"/>
-      <c r="AE3" s="96" t="s">
+      <c r="AD3" s="76"/>
+      <c r="AE3" s="75" t="s">
         <v>126</v>
       </c>
-      <c r="AF3" s="96" t="s">
+      <c r="AF3" s="75" t="s">
         <v>127</v>
       </c>
-      <c r="AG3" s="96" t="s">
+      <c r="AG3" s="75" t="s">
         <v>128</v>
       </c>
-      <c r="AH3" s="96" t="s">
+      <c r="AH3" s="75" t="s">
         <v>129</v>
       </c>
-      <c r="AI3" s="96" t="s">
+      <c r="AI3" s="75" t="s">
         <v>130</v>
       </c>
-      <c r="AJ3" s="97"/>
-      <c r="AK3" s="96" t="s">
+      <c r="AJ3" s="76"/>
+      <c r="AK3" s="75" t="s">
         <v>131</v>
       </c>
-      <c r="AL3" s="96" t="s">
+      <c r="AL3" s="75" t="s">
         <v>132</v>
       </c>
-      <c r="AM3" s="96" t="s">
+      <c r="AM3" s="75" t="s">
         <v>133</v>
       </c>
-      <c r="AN3" s="97"/>
-      <c r="AO3" s="97"/>
-      <c r="AP3" s="97"/>
-      <c r="AQ3" s="97"/>
-      <c r="AR3" s="97"/>
-      <c r="AS3" s="96" t="s">
+      <c r="AN3" s="76"/>
+      <c r="AO3" s="76"/>
+      <c r="AP3" s="76"/>
+      <c r="AQ3" s="76"/>
+      <c r="AR3" s="76"/>
+      <c r="AS3" s="75" t="s">
         <v>134</v>
       </c>
-      <c r="AT3" s="96" t="s">
+      <c r="AT3" s="75" t="s">
         <v>135</v>
       </c>
-      <c r="AU3" s="100" t="s">
+      <c r="AU3" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="AV3" s="96" t="s">
+      <c r="AV3" s="75" t="s">
         <v>137</v>
       </c>
-      <c r="AW3" s="97"/>
-      <c r="AX3" s="99"/>
+      <c r="AW3" s="76"/>
+      <c r="AX3" s="84"/>
       <c r="AY3" s="90"/>
       <c r="AZ3" s="90"/>
       <c r="BA3" s="90"/>
@@ -2340,60 +2340,60 @@
       <c r="EA3" s="1"/>
     </row>
     <row r="4" spans="1:131" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="107"/>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
       <c r="L4" s="3" t="s">
         <v>138</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="N4" s="97"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="97"/>
-      <c r="Q4" s="97"/>
-      <c r="R4" s="97"/>
-      <c r="S4" s="97"/>
-      <c r="T4" s="97"/>
-      <c r="U4" s="97"/>
-      <c r="V4" s="97"/>
-      <c r="W4" s="97"/>
-      <c r="X4" s="97"/>
-      <c r="Y4" s="97"/>
-      <c r="Z4" s="97"/>
-      <c r="AA4" s="97"/>
-      <c r="AB4" s="97"/>
-      <c r="AC4" s="97"/>
-      <c r="AD4" s="97"/>
-      <c r="AE4" s="97"/>
-      <c r="AF4" s="97"/>
-      <c r="AG4" s="97"/>
-      <c r="AH4" s="97"/>
-      <c r="AI4" s="97"/>
-      <c r="AJ4" s="97"/>
-      <c r="AK4" s="97"/>
-      <c r="AL4" s="97"/>
-      <c r="AM4" s="97"/>
-      <c r="AN4" s="97"/>
-      <c r="AO4" s="97"/>
-      <c r="AP4" s="97"/>
-      <c r="AQ4" s="97"/>
-      <c r="AR4" s="97"/>
-      <c r="AS4" s="97"/>
-      <c r="AT4" s="97"/>
-      <c r="AU4" s="101"/>
-      <c r="AV4" s="97"/>
-      <c r="AW4" s="97"/>
-      <c r="AX4" s="99"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76"/>
+      <c r="S4" s="76"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
+      <c r="V4" s="76"/>
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
+      <c r="Y4" s="76"/>
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="76"/>
+      <c r="AB4" s="76"/>
+      <c r="AC4" s="76"/>
+      <c r="AD4" s="76"/>
+      <c r="AE4" s="76"/>
+      <c r="AF4" s="76"/>
+      <c r="AG4" s="76"/>
+      <c r="AH4" s="76"/>
+      <c r="AI4" s="76"/>
+      <c r="AJ4" s="76"/>
+      <c r="AK4" s="76"/>
+      <c r="AL4" s="76"/>
+      <c r="AM4" s="76"/>
+      <c r="AN4" s="76"/>
+      <c r="AO4" s="76"/>
+      <c r="AP4" s="76"/>
+      <c r="AQ4" s="76"/>
+      <c r="AR4" s="76"/>
+      <c r="AS4" s="76"/>
+      <c r="AT4" s="76"/>
+      <c r="AU4" s="86"/>
+      <c r="AV4" s="76"/>
+      <c r="AW4" s="76"/>
+      <c r="AX4" s="84"/>
       <c r="AY4" s="87" t="s">
         <v>140</v>
       </c>
@@ -2404,24 +2404,24 @@
       <c r="BD4" s="88"/>
       <c r="BE4" s="88"/>
       <c r="BF4" s="88"/>
-      <c r="BG4" s="85" t="s">
+      <c r="BG4" s="97" t="s">
         <v>141</v>
       </c>
-      <c r="BH4" s="85"/>
+      <c r="BH4" s="97"/>
       <c r="BI4" s="11" t="s">
         <v>142</v>
       </c>
       <c r="BJ4" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="BK4" s="91" t="s">
+      <c r="BK4" s="92" t="s">
         <v>144</v>
       </c>
-      <c r="BL4" s="91"/>
-      <c r="BM4" s="92" t="s">
+      <c r="BL4" s="92"/>
+      <c r="BM4" s="93" t="s">
         <v>145</v>
       </c>
-      <c r="BN4" s="92"/>
+      <c r="BN4" s="93"/>
       <c r="BO4" s="12" t="s">
         <v>146</v>
       </c>
@@ -2615,70 +2615,70 @@
       <c r="AV5" s="3"/>
       <c r="AW5" s="3"/>
       <c r="AX5" s="14"/>
-      <c r="AY5" s="93" t="s">
+      <c r="AY5" s="94" t="s">
         <v>183</v>
       </c>
-      <c r="AZ5" s="94" t="s">
+      <c r="AZ5" s="95" t="s">
         <v>184</v>
       </c>
-      <c r="BA5" s="94" t="s">
+      <c r="BA5" s="95" t="s">
         <v>185</v>
       </c>
-      <c r="BB5" s="94" t="s">
+      <c r="BB5" s="95" t="s">
         <v>186</v>
       </c>
-      <c r="BC5" s="94" t="s">
+      <c r="BC5" s="95" t="s">
         <v>187</v>
       </c>
-      <c r="BD5" s="94" t="s">
+      <c r="BD5" s="95" t="s">
         <v>188</v>
       </c>
-      <c r="BE5" s="94" t="s">
+      <c r="BE5" s="95" t="s">
         <v>189</v>
       </c>
-      <c r="BF5" s="95" t="s">
+      <c r="BF5" s="96" t="s">
         <v>190</v>
       </c>
-      <c r="BG5" s="85" t="s">
+      <c r="BG5" s="97" t="s">
         <v>191</v>
       </c>
-      <c r="BH5" s="85" t="s">
+      <c r="BH5" s="97" t="s">
         <v>190</v>
       </c>
-      <c r="BI5" s="75" t="s">
+      <c r="BI5" s="98" t="s">
         <v>192</v>
       </c>
-      <c r="BJ5" s="75" t="s">
+      <c r="BJ5" s="98" t="s">
         <v>192</v>
       </c>
-      <c r="BK5" s="86" t="s">
+      <c r="BK5" s="107" t="s">
         <v>193</v>
       </c>
-      <c r="BL5" s="84" t="s">
+      <c r="BL5" s="91" t="s">
         <v>190</v>
       </c>
-      <c r="BM5" s="82" t="s">
+      <c r="BM5" s="105" t="s">
         <v>193</v>
       </c>
-      <c r="BN5" s="83" t="s">
+      <c r="BN5" s="106" t="s">
         <v>190</v>
       </c>
-      <c r="BO5" s="84" t="s">
+      <c r="BO5" s="91" t="s">
         <v>190</v>
       </c>
-      <c r="BP5" s="84" t="s">
+      <c r="BP5" s="91" t="s">
         <v>190</v>
       </c>
-      <c r="BQ5" s="75" t="s">
+      <c r="BQ5" s="98" t="s">
         <v>192</v>
       </c>
-      <c r="BR5" s="75" t="s">
+      <c r="BR5" s="98" t="s">
         <v>192</v>
       </c>
-      <c r="BS5" s="75" t="s">
+      <c r="BS5" s="98" t="s">
         <v>192</v>
       </c>
-      <c r="BT5" s="75" t="s">
+      <c r="BT5" s="98" t="s">
         <v>192</v>
       </c>
       <c r="BU5" s="1"/>
@@ -2892,28 +2892,28 @@
       <c r="AX6" s="14">
         <v>48</v>
       </c>
-      <c r="AY6" s="93"/>
-      <c r="AZ6" s="94"/>
-      <c r="BA6" s="94"/>
-      <c r="BB6" s="94"/>
-      <c r="BC6" s="94"/>
-      <c r="BD6" s="94"/>
-      <c r="BE6" s="94"/>
-      <c r="BF6" s="95"/>
-      <c r="BG6" s="85"/>
-      <c r="BH6" s="85"/>
-      <c r="BI6" s="75"/>
-      <c r="BJ6" s="75"/>
-      <c r="BK6" s="86"/>
-      <c r="BL6" s="84"/>
-      <c r="BM6" s="82"/>
-      <c r="BN6" s="83"/>
-      <c r="BO6" s="84"/>
-      <c r="BP6" s="84"/>
-      <c r="BQ6" s="75"/>
-      <c r="BR6" s="75"/>
-      <c r="BS6" s="75"/>
-      <c r="BT6" s="75"/>
+      <c r="AY6" s="94"/>
+      <c r="AZ6" s="95"/>
+      <c r="BA6" s="95"/>
+      <c r="BB6" s="95"/>
+      <c r="BC6" s="95"/>
+      <c r="BD6" s="95"/>
+      <c r="BE6" s="95"/>
+      <c r="BF6" s="96"/>
+      <c r="BG6" s="97"/>
+      <c r="BH6" s="97"/>
+      <c r="BI6" s="98"/>
+      <c r="BJ6" s="98"/>
+      <c r="BK6" s="107"/>
+      <c r="BL6" s="91"/>
+      <c r="BM6" s="105"/>
+      <c r="BN6" s="106"/>
+      <c r="BO6" s="91"/>
+      <c r="BP6" s="91"/>
+      <c r="BQ6" s="98"/>
+      <c r="BR6" s="98"/>
+      <c r="BS6" s="98"/>
+      <c r="BT6" s="98"/>
       <c r="BU6" s="1"/>
       <c r="BV6" s="1"/>
       <c r="BW6" s="1"/>
@@ -14751,7 +14751,7 @@
       <c r="EA51" s="1"/>
     </row>
     <row r="52" spans="1:131" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="76" t="s">
+      <c r="A52" s="99" t="s">
         <v>197</v>
       </c>
       <c r="B52" s="47" t="s">
@@ -15050,7 +15050,7 @@
       <c r="EA52" s="1"/>
     </row>
     <row r="53" spans="1:131" x14ac:dyDescent="0.25">
-      <c r="A53" s="77"/>
+      <c r="A53" s="100"/>
       <c r="B53" s="48" t="s">
         <v>199</v>
       </c>
@@ -15347,7 +15347,7 @@
       <c r="EA53" s="1"/>
     </row>
     <row r="54" spans="1:131" x14ac:dyDescent="0.25">
-      <c r="A54" s="77"/>
+      <c r="A54" s="100"/>
       <c r="B54" s="49"/>
       <c r="C54" s="1"/>
       <c r="D54" s="31"/>
@@ -15480,7 +15480,7 @@
       <c r="EA54" s="1"/>
     </row>
     <row r="55" spans="1:131" x14ac:dyDescent="0.25">
-      <c r="A55" s="77"/>
+      <c r="A55" s="100"/>
       <c r="B55" s="47" t="s">
         <v>200</v>
       </c>
@@ -15777,7 +15777,7 @@
       <c r="EA55" s="1"/>
     </row>
     <row r="56" spans="1:131" x14ac:dyDescent="0.25">
-      <c r="A56" s="77"/>
+      <c r="A56" s="100"/>
       <c r="B56" s="48" t="s">
         <v>201</v>
       </c>
@@ -16074,7 +16074,7 @@
       <c r="EA56" s="1"/>
     </row>
     <row r="57" spans="1:131" x14ac:dyDescent="0.25">
-      <c r="A57" s="77"/>
+      <c r="A57" s="100"/>
       <c r="B57" s="27"/>
       <c r="C57" s="1"/>
       <c r="D57" s="26"/>
@@ -16207,7 +16207,7 @@
       <c r="EA57" s="1"/>
     </row>
     <row r="58" spans="1:131" x14ac:dyDescent="0.25">
-      <c r="A58" s="77"/>
+      <c r="A58" s="100"/>
       <c r="B58" s="47" t="s">
         <v>202</v>
       </c>
@@ -16504,7 +16504,7 @@
       <c r="EA58" s="1"/>
     </row>
     <row r="59" spans="1:131" x14ac:dyDescent="0.25">
-      <c r="A59" s="78"/>
+      <c r="A59" s="101"/>
       <c r="B59" s="48" t="s">
         <v>203</v>
       </c>
@@ -18225,7 +18225,7 @@
     </row>
     <row r="67" spans="1:131" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
-      <c r="B67" s="79" t="s">
+      <c r="B67" s="102" t="s">
         <v>207</v>
       </c>
       <c r="C67" s="32"/>
@@ -18498,7 +18498,7 @@
     </row>
     <row r="68" spans="1:131" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
-      <c r="B68" s="80"/>
+      <c r="B68" s="103"/>
       <c r="C68" s="15"/>
       <c r="D68" s="36">
         <f>D38</f>
@@ -18769,7 +18769,7 @@
     </row>
     <row r="69" spans="1:131" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
-      <c r="B69" s="80"/>
+      <c r="B69" s="103"/>
       <c r="C69" s="15"/>
       <c r="D69" s="36">
         <f>D39</f>
@@ -19043,7 +19043,7 @@
     </row>
     <row r="70" spans="1:131" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-      <c r="B70" s="80"/>
+      <c r="B70" s="103"/>
       <c r="C70" s="15"/>
       <c r="D70" s="36">
         <f>D40</f>
@@ -19317,7 +19317,7 @@
     </row>
     <row r="71" spans="1:131" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
-      <c r="B71" s="81"/>
+      <c r="B71" s="104"/>
       <c r="C71" s="33"/>
       <c r="D71" s="33">
         <v>0</v>
@@ -34942,26 +34942,60 @@
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="K1:V1"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:N4"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="R2:R4"/>
-    <mergeCell ref="S2:S4"/>
-    <mergeCell ref="T2:T4"/>
-    <mergeCell ref="U2:U4"/>
-    <mergeCell ref="V2:V4"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="BT5:BT6"/>
+    <mergeCell ref="A52:A59"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="BM5:BM6"/>
+    <mergeCell ref="BN5:BN6"/>
+    <mergeCell ref="BO5:BO6"/>
+    <mergeCell ref="BP5:BP6"/>
+    <mergeCell ref="BQ5:BQ6"/>
+    <mergeCell ref="BR5:BR6"/>
+    <mergeCell ref="BG5:BG6"/>
+    <mergeCell ref="BH5:BH6"/>
+    <mergeCell ref="BI5:BI6"/>
+    <mergeCell ref="BJ5:BJ6"/>
+    <mergeCell ref="BK5:BK6"/>
+    <mergeCell ref="AY4:BF4"/>
+    <mergeCell ref="AY1:BS3"/>
+    <mergeCell ref="BL5:BL6"/>
+    <mergeCell ref="BK4:BL4"/>
+    <mergeCell ref="BM4:BN4"/>
+    <mergeCell ref="AY5:AY6"/>
+    <mergeCell ref="AZ5:AZ6"/>
+    <mergeCell ref="BA5:BA6"/>
+    <mergeCell ref="BB5:BB6"/>
+    <mergeCell ref="BC5:BC6"/>
+    <mergeCell ref="BD5:BD6"/>
+    <mergeCell ref="BE5:BE6"/>
+    <mergeCell ref="BF5:BF6"/>
+    <mergeCell ref="BG4:BH4"/>
+    <mergeCell ref="BS5:BS6"/>
+    <mergeCell ref="AR2:AR4"/>
+    <mergeCell ref="AS2:AV2"/>
+    <mergeCell ref="AW2:AW4"/>
+    <mergeCell ref="AX2:AX4"/>
+    <mergeCell ref="AP2:AP4"/>
+    <mergeCell ref="AQ2:AQ4"/>
+    <mergeCell ref="AS3:AS4"/>
+    <mergeCell ref="AT3:AT4"/>
+    <mergeCell ref="AU3:AU4"/>
+    <mergeCell ref="AV3:AV4"/>
+    <mergeCell ref="AM3:AM4"/>
+    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="AH3:AH4"/>
+    <mergeCell ref="AI3:AI4"/>
+    <mergeCell ref="AK3:AK4"/>
+    <mergeCell ref="AL3:AL4"/>
+    <mergeCell ref="AE2:AI2"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="W2:W4"/>
     <mergeCell ref="W1:AI1"/>
     <mergeCell ref="AJ1:AM1"/>
     <mergeCell ref="AN1:AQ1"/>
@@ -34978,60 +35012,26 @@
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="AN2:AN4"/>
     <mergeCell ref="AO2:AO4"/>
-    <mergeCell ref="AE2:AI2"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="AM3:AM4"/>
-    <mergeCell ref="AG3:AG4"/>
-    <mergeCell ref="AH3:AH4"/>
-    <mergeCell ref="AI3:AI4"/>
-    <mergeCell ref="AK3:AK4"/>
-    <mergeCell ref="AL3:AL4"/>
-    <mergeCell ref="AR2:AR4"/>
-    <mergeCell ref="AS2:AV2"/>
-    <mergeCell ref="AW2:AW4"/>
-    <mergeCell ref="AX2:AX4"/>
-    <mergeCell ref="AP2:AP4"/>
-    <mergeCell ref="AQ2:AQ4"/>
-    <mergeCell ref="AS3:AS4"/>
-    <mergeCell ref="AT3:AT4"/>
-    <mergeCell ref="AU3:AU4"/>
-    <mergeCell ref="AV3:AV4"/>
-    <mergeCell ref="AY4:BF4"/>
-    <mergeCell ref="AY1:BS3"/>
-    <mergeCell ref="BL5:BL6"/>
-    <mergeCell ref="BK4:BL4"/>
-    <mergeCell ref="BM4:BN4"/>
-    <mergeCell ref="AY5:AY6"/>
-    <mergeCell ref="AZ5:AZ6"/>
-    <mergeCell ref="BA5:BA6"/>
-    <mergeCell ref="BB5:BB6"/>
-    <mergeCell ref="BC5:BC6"/>
-    <mergeCell ref="BD5:BD6"/>
-    <mergeCell ref="BE5:BE6"/>
-    <mergeCell ref="BF5:BF6"/>
-    <mergeCell ref="BG4:BH4"/>
-    <mergeCell ref="BS5:BS6"/>
-    <mergeCell ref="BT5:BT6"/>
-    <mergeCell ref="A52:A59"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="BM5:BM6"/>
-    <mergeCell ref="BN5:BN6"/>
-    <mergeCell ref="BO5:BO6"/>
-    <mergeCell ref="BP5:BP6"/>
-    <mergeCell ref="BQ5:BQ6"/>
-    <mergeCell ref="BR5:BR6"/>
-    <mergeCell ref="BG5:BG6"/>
-    <mergeCell ref="BH5:BH6"/>
-    <mergeCell ref="BI5:BI6"/>
-    <mergeCell ref="BJ5:BJ6"/>
-    <mergeCell ref="BK5:BK6"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="K1:V1"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="R2:R4"/>
+    <mergeCell ref="S2:S4"/>
+    <mergeCell ref="T2:T4"/>
+    <mergeCell ref="U2:U4"/>
+    <mergeCell ref="V2:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:C48">
     <cfRule type="cellIs" dxfId="7" priority="10" stopIfTrue="1" operator="equal">

</xml_diff>